<commit_message>
Adjust Markov illustrative case to only have one generator
</commit_message>
<xml_diff>
--- a/data/markov/Power_ThermalGen.xlsx
+++ b/data/markov/Power_ThermalGen.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C5E558-08FE-4872-8DBE-ABF6849C30CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23748E3D-F0C3-4631-BA0E-FF64F8D3D12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50205" yWindow="-21690" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -114,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>Power - Thermal Generators</t>
   </si>
@@ -411,9 +424,6 @@
   </si>
   <si>
     <t>Gas</t>
-  </si>
-  <si>
-    <t>BaseLoadGenerator</t>
   </si>
   <si>
     <t>VariableGenerator</t>
@@ -872,13 +882,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1414,7 +1424,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>98</v>
@@ -1426,16 +1436,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="14">
-        <v>470.60700000000003</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="14">
         <v>200</v>
       </c>
       <c r="I8" s="14">
-        <v>470.60700000000003</v>
+        <v>200</v>
       </c>
       <c r="J8" s="14">
-        <v>470.60700000000003</v>
+        <v>200</v>
       </c>
       <c r="K8" s="13">
         <v>5</v>
@@ -1492,91 +1502,6 @@
         <v>96</v>
       </c>
       <c r="AE8" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="13">
-        <v>1</v>
-      </c>
-      <c r="G9" s="14">
-        <v>978</v>
-      </c>
-      <c r="H9" s="14">
-        <v>400</v>
-      </c>
-      <c r="I9" s="14">
-        <v>980.1</v>
-      </c>
-      <c r="J9" s="14">
-        <v>980.1</v>
-      </c>
-      <c r="K9" s="13">
-        <v>1</v>
-      </c>
-      <c r="L9" s="13">
-        <v>1</v>
-      </c>
-      <c r="M9" s="14">
-        <v>180</v>
-      </c>
-      <c r="N9" s="14">
-        <v>-180</v>
-      </c>
-      <c r="O9" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="P9" s="15">
-        <v>34.42340791738382</v>
-      </c>
-      <c r="Q9" s="15">
-        <v>0.43029259896729771</v>
-      </c>
-      <c r="R9" s="15">
-        <v>348.6</v>
-      </c>
-      <c r="S9" s="15">
-        <v>4.03</v>
-      </c>
-      <c r="T9" s="15">
-        <v>0</v>
-      </c>
-      <c r="U9" s="15"/>
-      <c r="V9" s="13">
-        <v>0</v>
-      </c>
-      <c r="W9" s="15">
-        <v>24781.499100000001</v>
-      </c>
-      <c r="X9" s="16">
-        <v>0.96</v>
-      </c>
-      <c r="Y9" s="17">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="18">
-        <v>46.77</v>
-      </c>
-      <c r="AC9" s="18">
-        <v>13.746700000000001</v>
-      </c>
-      <c r="AD9" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE9" s="19" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>